<commit_message>
Se realizo un revert.
Y se integro ya bien la columna de CRITERIO dentro del armado del archivo TIPO DE PROCESO
</commit_message>
<xml_diff>
--- a/archivos/HISTORIAL_PROCESOS.xlsx
+++ b/archivos/HISTORIAL_PROCESOS.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3095"/>
+  <dimension ref="A1:E3179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -66866,6 +66866,1846 @@
         </is>
       </c>
     </row>
+    <row r="3096">
+      <c r="A3096" t="n">
+        <v>2342118</v>
+      </c>
+      <c r="B3096" t="inlineStr">
+        <is>
+          <t>SIN NORMA</t>
+        </is>
+      </c>
+      <c r="C3096" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3096" t="inlineStr">
+        <is>
+          <t>SUDADERAS PARA MUJER DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3096" t="inlineStr"/>
+    </row>
+    <row r="3097">
+      <c r="A3097" t="n">
+        <v>2342119</v>
+      </c>
+      <c r="B3097" t="inlineStr">
+        <is>
+          <t>SIN NORMA</t>
+        </is>
+      </c>
+      <c r="C3097" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3097" t="inlineStr">
+        <is>
+          <t>SUDADERAS PARA MUJER DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3097" t="inlineStr"/>
+    </row>
+    <row r="3098">
+      <c r="A3098" t="n">
+        <v>2605174</v>
+      </c>
+      <c r="B3098" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3098" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3098" t="inlineStr">
+        <is>
+          <t>PANTALONES PARA NINA DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3098" t="inlineStr"/>
+    </row>
+    <row r="3099">
+      <c r="A3099" t="n">
+        <v>2605175</v>
+      </c>
+      <c r="B3099" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3099" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3099" t="inlineStr">
+        <is>
+          <t>PANTALONES PARA NINA DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3099" t="inlineStr"/>
+    </row>
+    <row r="3100">
+      <c r="A3100" t="n">
+        <v>2605176</v>
+      </c>
+      <c r="B3100" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3100" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3100" t="inlineStr">
+        <is>
+          <t>PANTALONES PARA NINA DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3100" t="inlineStr"/>
+    </row>
+    <row r="3101">
+      <c r="A3101" t="n">
+        <v>2730467</v>
+      </c>
+      <c r="B3101" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3101" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3101" t="inlineStr">
+        <is>
+          <t>PANTALONES CORTOS CENIDOS PARA MUJER DE FIBRAS SINTETICAS NO DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3101" t="inlineStr"/>
+    </row>
+    <row r="3102">
+      <c r="A3102" t="n">
+        <v>2901120</v>
+      </c>
+      <c r="B3102" t="inlineStr">
+        <is>
+          <t>SIN NORMA</t>
+        </is>
+      </c>
+      <c r="C3102" t="inlineStr">
+        <is>
+          <t>NOM-020-SCFI-1997</t>
+        </is>
+      </c>
+      <c r="D3102" t="inlineStr">
+        <is>
+          <t>CALZADO PARA HOMBRE O JOVEN CORTE SINTETICO SUELA SINTETICA</t>
+        </is>
+      </c>
+      <c r="E3102" t="inlineStr"/>
+    </row>
+    <row r="3103">
+      <c r="A3103" t="n">
+        <v>2901121</v>
+      </c>
+      <c r="B3103" t="inlineStr">
+        <is>
+          <t>SIN NORMA</t>
+        </is>
+      </c>
+      <c r="C3103" t="inlineStr">
+        <is>
+          <t>NOM-020-SCFI-1997</t>
+        </is>
+      </c>
+      <c r="D3103" t="inlineStr">
+        <is>
+          <t>CALZADO PARA HOMBRE O JOVEN CORTE SINTETICO SUELA SINTETICA</t>
+        </is>
+      </c>
+      <c r="E3103" t="inlineStr"/>
+    </row>
+    <row r="3104">
+      <c r="A3104" t="n">
+        <v>2901122</v>
+      </c>
+      <c r="B3104" t="inlineStr">
+        <is>
+          <t>SIN NORMA</t>
+        </is>
+      </c>
+      <c r="C3104" t="inlineStr">
+        <is>
+          <t>NOM-020-SCFI-1997</t>
+        </is>
+      </c>
+      <c r="D3104" t="inlineStr">
+        <is>
+          <t>CALZADO PARA HOMBRE O JOVEN CORTE SINTETICO SUELA SINTETICA</t>
+        </is>
+      </c>
+      <c r="E3104" t="inlineStr"/>
+    </row>
+    <row r="3105">
+      <c r="A3105" t="n">
+        <v>2901123</v>
+      </c>
+      <c r="B3105" t="inlineStr">
+        <is>
+          <t>SIN NORMA</t>
+        </is>
+      </c>
+      <c r="C3105" t="inlineStr">
+        <is>
+          <t>NOM-020-SCFI-1997</t>
+        </is>
+      </c>
+      <c r="D3105" t="inlineStr">
+        <is>
+          <t>CALZADO PARA HOMBRE O JOVEN CORTE SINTETICO SUELA SINTETICA</t>
+        </is>
+      </c>
+      <c r="E3105" t="inlineStr"/>
+    </row>
+    <row r="3106">
+      <c r="A3106" t="n">
+        <v>2901124</v>
+      </c>
+      <c r="B3106" t="inlineStr">
+        <is>
+          <t>SIN NORMA</t>
+        </is>
+      </c>
+      <c r="C3106" t="inlineStr">
+        <is>
+          <t>NOM-020-SCFI-1997</t>
+        </is>
+      </c>
+      <c r="D3106" t="inlineStr">
+        <is>
+          <t>CALZADO PARA HOMBRE O JOVEN CORTE SINTETICO SUELA SINTETICA</t>
+        </is>
+      </c>
+      <c r="E3106" t="inlineStr"/>
+    </row>
+    <row r="3107">
+      <c r="A3107" t="n">
+        <v>2901125</v>
+      </c>
+      <c r="B3107" t="inlineStr">
+        <is>
+          <t>SIN NORMA</t>
+        </is>
+      </c>
+      <c r="C3107" t="inlineStr">
+        <is>
+          <t>NOM-020-SCFI-1997</t>
+        </is>
+      </c>
+      <c r="D3107" t="inlineStr">
+        <is>
+          <t>CALZADO PARA HOMBRE O JOVEN CORTE SINTETICO SUELA SINTETICA</t>
+        </is>
+      </c>
+      <c r="E3107" t="inlineStr"/>
+    </row>
+    <row r="3108">
+      <c r="A3108" t="n">
+        <v>2901126</v>
+      </c>
+      <c r="B3108" t="inlineStr">
+        <is>
+          <t>SIN NORMA</t>
+        </is>
+      </c>
+      <c r="C3108" t="inlineStr">
+        <is>
+          <t>NOM-020-SCFI-1997</t>
+        </is>
+      </c>
+      <c r="D3108" t="inlineStr">
+        <is>
+          <t>CALZADO PARA HOMBRE O JOVEN CORTE SINTETICO SUELA SINTETICA</t>
+        </is>
+      </c>
+      <c r="E3108" t="inlineStr"/>
+    </row>
+    <row r="3109">
+      <c r="A3109" t="n">
+        <v>2901142</v>
+      </c>
+      <c r="B3109" t="inlineStr">
+        <is>
+          <t>SIN NORMA</t>
+        </is>
+      </c>
+      <c r="C3109" t="inlineStr">
+        <is>
+          <t>NOM-020-SCFI-1997</t>
+        </is>
+      </c>
+      <c r="D3109" t="inlineStr">
+        <is>
+          <t>CALZADO PARA HOMBRE O JOVEN CORTE SINTETICO SUELA SINTETICA</t>
+        </is>
+      </c>
+      <c r="E3109" t="inlineStr"/>
+    </row>
+    <row r="3110">
+      <c r="A3110" t="n">
+        <v>2901145</v>
+      </c>
+      <c r="B3110" t="inlineStr">
+        <is>
+          <t>SIN NORMA</t>
+        </is>
+      </c>
+      <c r="C3110" t="inlineStr">
+        <is>
+          <t>NOM-020-SCFI-1997</t>
+        </is>
+      </c>
+      <c r="D3110" t="inlineStr">
+        <is>
+          <t>CALZADO PARA HOMBRE O JOVEN CORTE SINTETICO SUELA SINTETICA</t>
+        </is>
+      </c>
+      <c r="E3110" t="inlineStr"/>
+    </row>
+    <row r="3111">
+      <c r="A3111" t="n">
+        <v>2901146</v>
+      </c>
+      <c r="B3111" t="inlineStr">
+        <is>
+          <t>SIN NORMA</t>
+        </is>
+      </c>
+      <c r="C3111" t="inlineStr">
+        <is>
+          <t>NOM-020-SCFI-1997</t>
+        </is>
+      </c>
+      <c r="D3111" t="inlineStr">
+        <is>
+          <t>CALZADO PARA HOMBRE O JOVEN CORTE SINTETICO SUELA SINTETICA</t>
+        </is>
+      </c>
+      <c r="E3111" t="inlineStr"/>
+    </row>
+    <row r="3112">
+      <c r="A3112" t="n">
+        <v>2956236</v>
+      </c>
+      <c r="B3112" t="inlineStr">
+        <is>
+          <t>SIN NORMA</t>
+        </is>
+      </c>
+      <c r="C3112" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3112" t="inlineStr">
+        <is>
+          <t>SUDADERAS PARA MUJER DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3112" t="inlineStr"/>
+    </row>
+    <row r="3113">
+      <c r="A3113" t="n">
+        <v>2956242</v>
+      </c>
+      <c r="B3113" t="inlineStr">
+        <is>
+          <t>SIN NORMA</t>
+        </is>
+      </c>
+      <c r="C3113" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3113" t="inlineStr">
+        <is>
+          <t>SUDADERAS PARA MUJER DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3113" t="inlineStr"/>
+    </row>
+    <row r="3114">
+      <c r="A3114" t="n">
+        <v>2956243</v>
+      </c>
+      <c r="B3114" t="inlineStr">
+        <is>
+          <t>SIN NORMA</t>
+        </is>
+      </c>
+      <c r="C3114" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3114" t="inlineStr">
+        <is>
+          <t>SUDADERAS PARA MUJER DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3114" t="inlineStr"/>
+    </row>
+    <row r="3115">
+      <c r="A3115" t="n">
+        <v>2956244</v>
+      </c>
+      <c r="B3115" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3115" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3115" t="inlineStr">
+        <is>
+          <t>SUDADERAS PARA MUJER DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3115" t="inlineStr"/>
+    </row>
+    <row r="3116">
+      <c r="A3116" t="n">
+        <v>2956245</v>
+      </c>
+      <c r="B3116" t="inlineStr">
+        <is>
+          <t>SIN NORMA</t>
+        </is>
+      </c>
+      <c r="C3116" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3116" t="inlineStr">
+        <is>
+          <t>SUDADERAS PARA MUJER DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3116" t="inlineStr"/>
+    </row>
+    <row r="3117">
+      <c r="A3117" t="n">
+        <v>2956246</v>
+      </c>
+      <c r="B3117" t="inlineStr">
+        <is>
+          <t>SIN NORMA</t>
+        </is>
+      </c>
+      <c r="C3117" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3117" t="inlineStr">
+        <is>
+          <t>SUDADERAS PARA MUJER DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3117" t="inlineStr"/>
+    </row>
+    <row r="3118">
+      <c r="A3118" t="n">
+        <v>4569194</v>
+      </c>
+      <c r="B3118" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3118" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3118" t="inlineStr">
+        <is>
+          <t>PLAYERAS PARA HOMBRE DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3118" t="inlineStr"/>
+    </row>
+    <row r="3119">
+      <c r="A3119" t="n">
+        <v>4569195</v>
+      </c>
+      <c r="B3119" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3119" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3119" t="inlineStr">
+        <is>
+          <t>PLAYERAS PARA HOMBRE DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3119" t="inlineStr"/>
+    </row>
+    <row r="3120">
+      <c r="A3120" t="n">
+        <v>4569196</v>
+      </c>
+      <c r="B3120" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3120" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3120" t="inlineStr">
+        <is>
+          <t>PLAYERAS PARA HOMBRE DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3120" t="inlineStr"/>
+    </row>
+    <row r="3121">
+      <c r="A3121" t="n">
+        <v>4569197</v>
+      </c>
+      <c r="B3121" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3121" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3121" t="inlineStr">
+        <is>
+          <t>PLAYERAS PARA HOMBRE DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3121" t="inlineStr"/>
+    </row>
+    <row r="3122">
+      <c r="A3122" t="n">
+        <v>4569198</v>
+      </c>
+      <c r="B3122" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3122" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3122" t="inlineStr">
+        <is>
+          <t>PLAYERAS PARA HOMBRE DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3122" t="inlineStr"/>
+    </row>
+    <row r="3123">
+      <c r="A3123" t="n">
+        <v>4744483</v>
+      </c>
+      <c r="B3123" t="inlineStr">
+        <is>
+          <t>SIN NORMA</t>
+        </is>
+      </c>
+      <c r="C3123" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3123" t="inlineStr">
+        <is>
+          <t>PLAYERAS PARA MUJER DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3123" t="inlineStr"/>
+    </row>
+    <row r="3124">
+      <c r="A3124" t="n">
+        <v>4838669</v>
+      </c>
+      <c r="B3124" t="inlineStr">
+        <is>
+          <t>SIN NORMA</t>
+        </is>
+      </c>
+      <c r="C3124" t="inlineStr">
+        <is>
+          <t>NOM-020-SCFI-1997</t>
+        </is>
+      </c>
+      <c r="D3124" t="inlineStr">
+        <is>
+          <t>CALZADO PARA MUJER O JOVENCITA CORTE TEXTIL SUELA SINTETICA</t>
+        </is>
+      </c>
+      <c r="E3124" t="inlineStr"/>
+    </row>
+    <row r="3125">
+      <c r="A3125" t="n">
+        <v>4838670</v>
+      </c>
+      <c r="B3125" t="inlineStr">
+        <is>
+          <t>SIN NORMA</t>
+        </is>
+      </c>
+      <c r="C3125" t="inlineStr">
+        <is>
+          <t>NOM-020-SCFI-1997</t>
+        </is>
+      </c>
+      <c r="D3125" t="inlineStr">
+        <is>
+          <t>CALZADO PARA MUJER O JOVENCITA CORTE TEXTIL SUELA SINTETICA</t>
+        </is>
+      </c>
+      <c r="E3125" t="inlineStr"/>
+    </row>
+    <row r="3126">
+      <c r="A3126" t="n">
+        <v>4838671</v>
+      </c>
+      <c r="B3126" t="inlineStr">
+        <is>
+          <t>SIN NORMA</t>
+        </is>
+      </c>
+      <c r="C3126" t="inlineStr">
+        <is>
+          <t>NOM-020-SCFI-1997</t>
+        </is>
+      </c>
+      <c r="D3126" t="inlineStr">
+        <is>
+          <t>CALZADO PARA MUJER O JOVENCITA CORTE TEXTIL SUELA SINTETICA</t>
+        </is>
+      </c>
+      <c r="E3126" t="inlineStr"/>
+    </row>
+    <row r="3127">
+      <c r="A3127" t="n">
+        <v>4838672</v>
+      </c>
+      <c r="B3127" t="inlineStr">
+        <is>
+          <t>SIN NORMA</t>
+        </is>
+      </c>
+      <c r="C3127" t="inlineStr">
+        <is>
+          <t>NOM-020-SCFI-1997</t>
+        </is>
+      </c>
+      <c r="D3127" t="inlineStr">
+        <is>
+          <t>CALZADO PARA MUJER O JOVENCITA CORTE TEXTIL SUELA SINTETICA</t>
+        </is>
+      </c>
+      <c r="E3127" t="inlineStr"/>
+    </row>
+    <row r="3128">
+      <c r="A3128" t="n">
+        <v>4925306</v>
+      </c>
+      <c r="B3128" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3128" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3128" t="inlineStr">
+        <is>
+          <t>PLAYERAS PARA MUJER DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3128" t="inlineStr"/>
+    </row>
+    <row r="3129">
+      <c r="A3129" t="n">
+        <v>5206104</v>
+      </c>
+      <c r="B3129" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3129" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3129" t="inlineStr">
+        <is>
+          <t>BANADORES PARA NINA DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3129" t="inlineStr"/>
+    </row>
+    <row r="3130">
+      <c r="A3130" t="n">
+        <v>5255916</v>
+      </c>
+      <c r="B3130" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3130" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3130" t="inlineStr">
+        <is>
+          <t>BANADORES PARA MUJER DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3130" t="inlineStr"/>
+    </row>
+    <row r="3131">
+      <c r="A3131" t="n">
+        <v>5255917</v>
+      </c>
+      <c r="B3131" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3131" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3131" t="inlineStr">
+        <is>
+          <t>BANADORES PARA MUJER DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3131" t="inlineStr"/>
+    </row>
+    <row r="3132">
+      <c r="A3132" t="n">
+        <v>5255918</v>
+      </c>
+      <c r="B3132" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3132" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3132" t="inlineStr">
+        <is>
+          <t>BANADORES PARA MUJER DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3132" t="inlineStr"/>
+    </row>
+    <row r="3133">
+      <c r="A3133" t="n">
+        <v>5255920</v>
+      </c>
+      <c r="B3133" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3133" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3133" t="inlineStr">
+        <is>
+          <t>BANADORES PARA MUJER DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3133" t="inlineStr"/>
+    </row>
+    <row r="3134">
+      <c r="A3134" t="n">
+        <v>5255921</v>
+      </c>
+      <c r="B3134" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3134" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3134" t="inlineStr">
+        <is>
+          <t>BANADORES PARA MUJER DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3134" t="inlineStr"/>
+    </row>
+    <row r="3135">
+      <c r="A3135" t="n">
+        <v>5255922</v>
+      </c>
+      <c r="B3135" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3135" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3135" t="inlineStr">
+        <is>
+          <t>BANADORES PARA MUJER DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3135" t="inlineStr"/>
+    </row>
+    <row r="3136">
+      <c r="A3136" t="n">
+        <v>2923828</v>
+      </c>
+      <c r="B3136" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3136" t="inlineStr">
+        <is>
+          <t>NOM-050-SCFI-2004, NOM-133/3-SCFI-1999</t>
+        </is>
+      </c>
+      <c r="D3136" t="inlineStr">
+        <is>
+          <t>MUEBLES DE METAL (CAMAS PLEGABLES)</t>
+        </is>
+      </c>
+      <c r="E3136" t="inlineStr"/>
+    </row>
+    <row r="3137">
+      <c r="A3137" t="n">
+        <v>4767344</v>
+      </c>
+      <c r="B3137" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3137" t="inlineStr">
+        <is>
+          <t>NOM-050-SCFI-2004</t>
+        </is>
+      </c>
+      <c r="D3137" t="inlineStr">
+        <is>
+          <t>SILLAS DE METAL</t>
+        </is>
+      </c>
+      <c r="E3137" t="inlineStr"/>
+    </row>
+    <row r="3138">
+      <c r="A3138" t="n">
+        <v>4767347</v>
+      </c>
+      <c r="B3138" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3138" t="inlineStr">
+        <is>
+          <t>NOM-050-SCFI-2004, NOM-133/3-SCFI-1999</t>
+        </is>
+      </c>
+      <c r="D3138" t="inlineStr">
+        <is>
+          <t>MUEBLES DE MADERA</t>
+        </is>
+      </c>
+      <c r="E3138" t="inlineStr"/>
+    </row>
+    <row r="3139">
+      <c r="A3139" t="n">
+        <v>4899301</v>
+      </c>
+      <c r="B3139" t="inlineStr">
+        <is>
+          <t>ADHERIBLE</t>
+        </is>
+      </c>
+      <c r="C3139" t="inlineStr">
+        <is>
+          <t>NOM-050-SCFI-2004</t>
+        </is>
+      </c>
+      <c r="D3139" t="inlineStr">
+        <is>
+          <t>RAQUETAS CON ACCESORIOS</t>
+        </is>
+      </c>
+      <c r="E3139" t="inlineStr"/>
+    </row>
+    <row r="3140">
+      <c r="A3140" t="n">
+        <v>4682887</v>
+      </c>
+      <c r="B3140" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3140" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3140" t="inlineStr">
+        <is>
+          <t>CHALECOS SALVAVIDAS</t>
+        </is>
+      </c>
+      <c r="E3140" t="inlineStr"/>
+    </row>
+    <row r="3141">
+      <c r="A3141" t="n">
+        <v>712813</v>
+      </c>
+      <c r="B3141" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3141" t="inlineStr">
+        <is>
+          <t>NOM-015-SCFI-2007, NOM-050-SCFI-2004</t>
+        </is>
+      </c>
+      <c r="D3141" t="inlineStr">
+        <is>
+          <t>JUEGO DE 2 ARTICULOS PARA CULTURA FISICA</t>
+        </is>
+      </c>
+      <c r="E3141" t="inlineStr"/>
+    </row>
+    <row r="3142">
+      <c r="A3142" t="n">
+        <v>2895786</v>
+      </c>
+      <c r="B3142" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3142" t="inlineStr">
+        <is>
+          <t>NOM-002-CONAGUA-2021, NOM-050-SCFI-2004</t>
+        </is>
+      </c>
+      <c r="D3142" t="inlineStr">
+        <is>
+          <t>COLCHONES INFLABLES DE PLASTICO</t>
+        </is>
+      </c>
+      <c r="E3142" t="inlineStr"/>
+    </row>
+    <row r="3143">
+      <c r="A3143" t="n">
+        <v>2745730</v>
+      </c>
+      <c r="B3143" t="inlineStr">
+        <is>
+          <t>ADHERIBLE</t>
+        </is>
+      </c>
+      <c r="C3143" t="inlineStr">
+        <is>
+          <t>NOM-015-SCFI-2007</t>
+        </is>
+      </c>
+      <c r="D3143" t="inlineStr">
+        <is>
+          <t>BALONES INFLABLES</t>
+        </is>
+      </c>
+      <c r="E3143" t="inlineStr"/>
+    </row>
+    <row r="3144">
+      <c r="A3144" t="n">
+        <v>4232397</v>
+      </c>
+      <c r="B3144" t="inlineStr">
+        <is>
+          <t>ADHERIBLE</t>
+        </is>
+      </c>
+      <c r="C3144" t="inlineStr">
+        <is>
+          <t>NOM-015-SCFI-2007</t>
+        </is>
+      </c>
+      <c r="D3144" t="inlineStr">
+        <is>
+          <t>BALONES INFLABLES</t>
+        </is>
+      </c>
+      <c r="E3144" t="inlineStr"/>
+    </row>
+    <row r="3145">
+      <c r="A3145" t="n">
+        <v>5183785</v>
+      </c>
+      <c r="B3145" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3145" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3145" t="inlineStr">
+        <is>
+          <t>GORRAS</t>
+        </is>
+      </c>
+      <c r="E3145" t="inlineStr"/>
+    </row>
+    <row r="3146">
+      <c r="A3146" t="n">
+        <v>2648470</v>
+      </c>
+      <c r="B3146" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3146" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3146" t="inlineStr">
+        <is>
+          <t>SOMBREROS</t>
+        </is>
+      </c>
+      <c r="E3146" t="inlineStr"/>
+    </row>
+    <row r="3147">
+      <c r="A3147" t="n">
+        <v>4667088</v>
+      </c>
+      <c r="B3147" t="inlineStr">
+        <is>
+          <t>ADHERIBLE</t>
+        </is>
+      </c>
+      <c r="C3147" t="inlineStr">
+        <is>
+          <t>NOM-015-SCFI-2007</t>
+        </is>
+      </c>
+      <c r="D3147" t="inlineStr">
+        <is>
+          <t>BALONES INFLABLES</t>
+        </is>
+      </c>
+      <c r="E3147" t="inlineStr"/>
+    </row>
+    <row r="3148">
+      <c r="A3148" t="n">
+        <v>2630622</v>
+      </c>
+      <c r="B3148" t="inlineStr">
+        <is>
+          <t>ADHERIBLE</t>
+        </is>
+      </c>
+      <c r="C3148" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3148" t="inlineStr">
+        <is>
+          <t>JUEGO DE 3 PARES DE CALCETINES DE ALGODON DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3148" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3149">
+      <c r="A3149" t="n">
+        <v>2630629</v>
+      </c>
+      <c r="B3149" t="inlineStr">
+        <is>
+          <t>ADHERIBLE</t>
+        </is>
+      </c>
+      <c r="C3149" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3149" t="inlineStr">
+        <is>
+          <t>JUEGO DE 3 PARES DE CALCETINES DE ALGODON DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3149" t="inlineStr"/>
+    </row>
+    <row r="3150">
+      <c r="A3150" t="n">
+        <v>2308152</v>
+      </c>
+      <c r="B3150" t="inlineStr">
+        <is>
+          <t>ADHERIBLE</t>
+        </is>
+      </c>
+      <c r="C3150" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3150" t="inlineStr">
+        <is>
+          <t>JUEGO DE 3 PARES DE CALCETINES DE ALGODON DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3150" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3151">
+      <c r="A3151" t="n">
+        <v>2308195</v>
+      </c>
+      <c r="B3151" t="inlineStr">
+        <is>
+          <t>ADHERIBLE</t>
+        </is>
+      </c>
+      <c r="C3151" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3151" t="inlineStr">
+        <is>
+          <t>JUEGO DE 3 PARES DE CALCETINES DE ALGODON DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3151" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3152">
+      <c r="A3152" t="n">
+        <v>2461442</v>
+      </c>
+      <c r="B3152" t="inlineStr">
+        <is>
+          <t>ADHERIBLE</t>
+        </is>
+      </c>
+      <c r="C3152" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3152" t="inlineStr">
+        <is>
+          <t>CALCETINES DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3152" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3153">
+      <c r="A3153" t="n">
+        <v>2172064</v>
+      </c>
+      <c r="B3153" t="inlineStr">
+        <is>
+          <t>ADHERIBLE</t>
+        </is>
+      </c>
+      <c r="C3153" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3153" t="inlineStr">
+        <is>
+          <t>JUEGO DE 3 PARES DE CALCETINES DE ALGODON DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3153" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3154">
+      <c r="A3154" t="n">
+        <v>1862929</v>
+      </c>
+      <c r="B3154" t="inlineStr">
+        <is>
+          <t>ADHERIBLE</t>
+        </is>
+      </c>
+      <c r="C3154" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3154" t="inlineStr">
+        <is>
+          <t>CALCETINES DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3154" t="inlineStr"/>
+    </row>
+    <row r="3155">
+      <c r="A3155" t="n">
+        <v>1862927</v>
+      </c>
+      <c r="B3155" t="inlineStr">
+        <is>
+          <t>ADHERIBLE</t>
+        </is>
+      </c>
+      <c r="C3155" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3155" t="inlineStr">
+        <is>
+          <t>CALCETINES DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3155" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3156">
+      <c r="A3156" t="n">
+        <v>2461443</v>
+      </c>
+      <c r="B3156" t="inlineStr">
+        <is>
+          <t>ADHERIBLE</t>
+        </is>
+      </c>
+      <c r="C3156" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3156" t="inlineStr">
+        <is>
+          <t>CALCETINES DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3156" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3157">
+      <c r="A3157" t="n">
+        <v>2308148</v>
+      </c>
+      <c r="B3157" t="inlineStr">
+        <is>
+          <t>ADHERIBLE</t>
+        </is>
+      </c>
+      <c r="C3157" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3157" t="inlineStr">
+        <is>
+          <t>JUEGO DE 3 PARES DE CALCETINES DE ALGODON DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3157" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3158">
+      <c r="A3158" t="n">
+        <v>2308147</v>
+      </c>
+      <c r="B3158" t="inlineStr">
+        <is>
+          <t>ADHERIBLE</t>
+        </is>
+      </c>
+      <c r="C3158" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3158" t="inlineStr">
+        <is>
+          <t>JUEGO DE 3 PARES DE CALCETINES DE ALGODON DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3158" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3159">
+      <c r="A3159" t="n">
+        <v>2308146</v>
+      </c>
+      <c r="B3159" t="inlineStr">
+        <is>
+          <t>ADHERIBLE</t>
+        </is>
+      </c>
+      <c r="C3159" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3159" t="inlineStr">
+        <is>
+          <t>JUEGO DE 3 PARES DE CALCETINES DE ALGODON DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3159" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3160">
+      <c r="A3160" t="n">
+        <v>2308218</v>
+      </c>
+      <c r="B3160" t="inlineStr">
+        <is>
+          <t>ADHERIBLE</t>
+        </is>
+      </c>
+      <c r="C3160" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3160" t="inlineStr">
+        <is>
+          <t>JUEGO DE 3 PARES DE CALCETINES DE ALGODON DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3160" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3161">
+      <c r="A3161" t="n">
+        <v>2415065</v>
+      </c>
+      <c r="B3161" t="inlineStr">
+        <is>
+          <t>ADHERIBLE</t>
+        </is>
+      </c>
+      <c r="C3161" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3161" t="inlineStr">
+        <is>
+          <t>JUEGO DE 3 PARES DE CALCETINES DE ALGODON DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3161" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3162">
+      <c r="A3162" t="n">
+        <v>2172052</v>
+      </c>
+      <c r="B3162" t="inlineStr">
+        <is>
+          <t>ADHERIBLE</t>
+        </is>
+      </c>
+      <c r="C3162" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3162" t="inlineStr">
+        <is>
+          <t>JUEGO DE 3 PARES DE CALCETINES DE ALGODON DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3162" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3163">
+      <c r="A3163" t="n">
+        <v>2172051</v>
+      </c>
+      <c r="B3163" t="inlineStr">
+        <is>
+          <t>ADHERIBLE</t>
+        </is>
+      </c>
+      <c r="C3163" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3163" t="inlineStr">
+        <is>
+          <t>JUEGO DE 3 PARES DE CALCETINES DE ALGODON DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3163" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3164">
+      <c r="A3164" t="n">
+        <v>5085164</v>
+      </c>
+      <c r="B3164" t="inlineStr">
+        <is>
+          <t>ADHERIBLE</t>
+        </is>
+      </c>
+      <c r="C3164" t="inlineStr">
+        <is>
+          <t>NOM-015-SCFI-2007</t>
+        </is>
+      </c>
+      <c r="D3164" t="inlineStr">
+        <is>
+          <t>BALONES INFLABLES</t>
+        </is>
+      </c>
+      <c r="E3164" t="inlineStr"/>
+    </row>
+    <row r="3165">
+      <c r="A3165" t="n">
+        <v>4714062</v>
+      </c>
+      <c r="B3165" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3165" t="inlineStr">
+        <is>
+          <t>NOM-050-SCFI-2004</t>
+        </is>
+      </c>
+      <c r="D3165" t="inlineStr">
+        <is>
+          <t>JUEGO DE PELOTAS</t>
+        </is>
+      </c>
+      <c r="E3165" t="inlineStr"/>
+    </row>
+    <row r="3166">
+      <c r="A3166" t="n">
+        <v>4714185</v>
+      </c>
+      <c r="B3166" t="inlineStr">
+        <is>
+          <t>ADHERIBLE</t>
+        </is>
+      </c>
+      <c r="C3166" t="inlineStr">
+        <is>
+          <t>NOM-050-SCFI-2004</t>
+        </is>
+      </c>
+      <c r="D3166" t="inlineStr">
+        <is>
+          <t>JUEGO DE PELOTAS</t>
+        </is>
+      </c>
+      <c r="E3166" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3167">
+      <c r="A3167" t="n">
+        <v>4852464</v>
+      </c>
+      <c r="B3167" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3167" t="inlineStr">
+        <is>
+          <t>NOM-015-SCFI-2007, NOM-050-SCFI-2004</t>
+        </is>
+      </c>
+      <c r="D3167" t="inlineStr">
+        <is>
+          <t>ARTICULOS PARA YOGA</t>
+        </is>
+      </c>
+      <c r="E3167" t="inlineStr"/>
+    </row>
+    <row r="3168">
+      <c r="A3168" t="n">
+        <v>712811</v>
+      </c>
+      <c r="B3168" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3168" t="inlineStr">
+        <is>
+          <t>NOM-015-SCFI-2007, NOM-050-SCFI-2004</t>
+        </is>
+      </c>
+      <c r="D3168" t="inlineStr">
+        <is>
+          <t>JUEGO DE ARTICULOS PARA CULTURA FISICA</t>
+        </is>
+      </c>
+      <c r="E3168" t="inlineStr"/>
+    </row>
+    <row r="3169">
+      <c r="A3169" t="n">
+        <v>712790</v>
+      </c>
+      <c r="B3169" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3169" t="inlineStr">
+        <is>
+          <t>NOM-015-SCFI-2007, NOM-050-SCFI-2004</t>
+        </is>
+      </c>
+      <c r="D3169" t="inlineStr">
+        <is>
+          <t>JUEGO DE 2 MANCUERNAS</t>
+        </is>
+      </c>
+      <c r="E3169" t="inlineStr"/>
+    </row>
+    <row r="3170">
+      <c r="A3170" t="n">
+        <v>2722539</v>
+      </c>
+      <c r="B3170" t="inlineStr">
+        <is>
+          <t>COSTURA</t>
+        </is>
+      </c>
+      <c r="C3170" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3170" t="inlineStr">
+        <is>
+          <t>CHALECOS SALVAVIDAS</t>
+        </is>
+      </c>
+      <c r="E3170" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3171">
+      <c r="A3171" t="n">
+        <v>2722538</v>
+      </c>
+      <c r="B3171" t="inlineStr">
+        <is>
+          <t>COSTURA</t>
+        </is>
+      </c>
+      <c r="C3171" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3171" t="inlineStr">
+        <is>
+          <t>CHALECOS SALVAVIDAS</t>
+        </is>
+      </c>
+      <c r="E3171" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3172">
+      <c r="A3172" t="n">
+        <v>2722537</v>
+      </c>
+      <c r="B3172" t="inlineStr">
+        <is>
+          <t>COSTURA</t>
+        </is>
+      </c>
+      <c r="C3172" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3172" t="inlineStr">
+        <is>
+          <t>CHALECOS SALVAVIDAS</t>
+        </is>
+      </c>
+      <c r="E3172" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3173">
+      <c r="A3173" t="n">
+        <v>2722536</v>
+      </c>
+      <c r="B3173" t="inlineStr">
+        <is>
+          <t>COSTURA</t>
+        </is>
+      </c>
+      <c r="C3173" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021</t>
+        </is>
+      </c>
+      <c r="D3173" t="inlineStr">
+        <is>
+          <t>CHALECOS SALVAVIDAS</t>
+        </is>
+      </c>
+      <c r="E3173" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3174">
+      <c r="A3174" t="n">
+        <v>1446242</v>
+      </c>
+      <c r="B3174" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3174" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021, NOM-020-SCFI-1997</t>
+        </is>
+      </c>
+      <c r="D3174" t="inlineStr">
+        <is>
+          <t>MALETAS CON LA SUPERFICIE EXTERIOR DE MATERIA TEXTIL</t>
+        </is>
+      </c>
+      <c r="E3174" t="inlineStr"/>
+    </row>
+    <row r="3175">
+      <c r="A3175" t="n">
+        <v>5045657</v>
+      </c>
+      <c r="B3175" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3175" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021, NOM-020-SCFI-1997</t>
+        </is>
+      </c>
+      <c r="D3175" t="inlineStr">
+        <is>
+          <t>MOCHILAS CON LA SUPERFICIE EXTERIOR DE MATERIA TEXTIL</t>
+        </is>
+      </c>
+      <c r="E3175" t="inlineStr"/>
+    </row>
+    <row r="3176">
+      <c r="A3176" t="n">
+        <v>4108229</v>
+      </c>
+      <c r="B3176" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3176" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021, NOM-015-SCFI-2007</t>
+        </is>
+      </c>
+      <c r="D3176" t="inlineStr">
+        <is>
+          <t>PLAYERAS PARA HOMBRE DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3176" t="inlineStr"/>
+    </row>
+    <row r="3177">
+      <c r="A3177" t="n">
+        <v>4108228</v>
+      </c>
+      <c r="B3177" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3177" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021, NOM-015-SCFI-2007</t>
+        </is>
+      </c>
+      <c r="D3177" t="inlineStr">
+        <is>
+          <t>PLAYERAS PARA HOMBRE DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3177" t="inlineStr"/>
+    </row>
+    <row r="3178">
+      <c r="A3178" t="n">
+        <v>4108227</v>
+      </c>
+      <c r="B3178" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3178" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021, NOM-015-SCFI-2007</t>
+        </is>
+      </c>
+      <c r="D3178" t="inlineStr">
+        <is>
+          <t>PLAYERAS PARA HOMBRE DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3178" t="inlineStr"/>
+    </row>
+    <row r="3179">
+      <c r="A3179" t="n">
+        <v>4108226</v>
+      </c>
+      <c r="B3179" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3179" t="inlineStr">
+        <is>
+          <t>NOM-004-SE-2021, NOM-015-SCFI-2007</t>
+        </is>
+      </c>
+      <c r="D3179" t="inlineStr">
+        <is>
+          <t>PLAYERAS PARA HOMBRE DE FIBRAS SINTETICAS DE PUNTO</t>
+        </is>
+      </c>
+      <c r="E3179" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nueva version de la aplicacion con eleccion de archivos y exportacion de excel
</commit_message>
<xml_diff>
--- a/archivos/HISTORIAL_PROCESOS.xlsx
+++ b/archivos/HISTORIAL_PROCESOS.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3179"/>
+  <dimension ref="A1:E3180"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -68706,6 +68706,27 @@
       </c>
       <c r="E3179" t="inlineStr"/>
     </row>
+    <row r="3180">
+      <c r="A3180" t="n">
+        <v>444444</v>
+      </c>
+      <c r="B3180" t="inlineStr">
+        <is>
+          <t>ADHERIBLE</t>
+        </is>
+      </c>
+      <c r="C3180" t="inlineStr">
+        <is>
+          <t>NOM-050-SCFI-2004</t>
+        </is>
+      </c>
+      <c r="D3180" t="inlineStr">
+        <is>
+          <t>BASTON DE SENDERISMO</t>
+        </is>
+      </c>
+      <c r="E3180" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>